<commit_message>
W9 mandatory, free camera added
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Status</t>
   </si>
@@ -135,13 +135,28 @@
   </si>
   <si>
     <t>customise later</t>
+  </si>
+  <si>
+    <t>add texture</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>Anna Nguyen</t>
+  </si>
+  <si>
+    <t>https://github.com/anguyen10/Roll-A-Ball</t>
+  </si>
+  <si>
+    <t>get the player and camera to sync</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -179,6 +194,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -290,10 +312,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -383,8 +406,13 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -497,7 +525,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,7 +533,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,11 +553,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2422,8 +2450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2458,7 +2486,9 @@
       <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="30" t="s">
+        <v>39</v>
+      </c>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
       <c r="G4" s="32"/>
@@ -2469,7 +2499,9 @@
       <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="33" t="s">
+        <v>40</v>
+      </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
@@ -2486,7 +2518,7 @@
       </c>
       <c r="D7" s="9">
         <f>COUNTIFS(J12:J15,TRUE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -2495,7 +2527,7 @@
       </c>
       <c r="D8" s="9">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2504,7 +2536,7 @@
       </c>
       <c r="D9" s="24">
         <f>K39</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2563,11 +2595,13 @@
       <c r="E13" s="8"/>
       <c r="F13" s="7" t="str">
         <f>IF(J13,"Done","To Be Done")</f>
-        <v>To Be Done</v>
-      </c>
-      <c r="G13" s="19"/>
+        <v>Done</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="J13" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2583,11 +2617,13 @@
       <c r="E14" s="8"/>
       <c r="F14" s="7" t="str">
         <f>IF(J14,"Done","To Be Done")</f>
-        <v>To Be Done</v>
-      </c>
-      <c r="G14" s="19"/>
+        <v>Done</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>38</v>
+      </c>
       <c r="J14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2603,11 +2639,13 @@
       <c r="E15" s="8"/>
       <c r="F15" s="7" t="str">
         <f>IF(J15,"Done","To Be Done")</f>
-        <v>To Be Done</v>
-      </c>
-      <c r="G15" s="19"/>
+        <v>Done</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>38</v>
+      </c>
       <c r="J15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3053,17 +3091,17 @@
       <c r="E34" s="8"/>
       <c r="F34" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G34" s="19">
-        <v>0</v>
+        <v>Done</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="J34" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
@@ -3165,7 +3203,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3198,16 +3236,19 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId4" name="Check Box 11">
+            <control shapeId="1035" r:id="rId5" name="Check Box 11">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3229,7 +3270,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId5" name="Check Box 12">
+            <control shapeId="1036" r:id="rId6" name="Check Box 12">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3251,7 +3292,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId6" name="Check Box 13">
+            <control shapeId="1037" r:id="rId7" name="Check Box 13">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3273,7 +3314,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId7" name="Check Box 14">
+            <control shapeId="1038" r:id="rId8" name="Check Box 14">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3295,7 +3336,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1054" r:id="rId8" name="Check Box 30">
+            <control shapeId="1054" r:id="rId9" name="Check Box 30">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3317,7 +3358,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1055" r:id="rId9" name="Check Box 31">
+            <control shapeId="1055" r:id="rId10" name="Check Box 31">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3339,7 +3380,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1056" r:id="rId10" name="Check Box 32">
+            <control shapeId="1056" r:id="rId11" name="Check Box 32">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3361,7 +3402,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1057" r:id="rId11" name="Check Box 33">
+            <control shapeId="1057" r:id="rId12" name="Check Box 33">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3383,7 +3424,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1059" r:id="rId12" name="Check Box 35">
+            <control shapeId="1059" r:id="rId13" name="Check Box 35">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3405,7 +3446,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1060" r:id="rId13" name="Check Box 36">
+            <control shapeId="1060" r:id="rId14" name="Check Box 36">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3427,7 +3468,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1062" r:id="rId14" name="Check Box 38">
+            <control shapeId="1062" r:id="rId15" name="Check Box 38">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3449,7 +3490,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1063" r:id="rId15" name="Check Box 39">
+            <control shapeId="1063" r:id="rId16" name="Check Box 39">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3471,7 +3512,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1065" r:id="rId16" name="Check Box 41">
+            <control shapeId="1065" r:id="rId17" name="Check Box 41">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3493,7 +3534,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1066" r:id="rId17" name="Check Box 42">
+            <control shapeId="1066" r:id="rId18" name="Check Box 42">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3515,7 +3556,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1067" r:id="rId18" name="Check Box 43">
+            <control shapeId="1067" r:id="rId19" name="Check Box 43">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3537,7 +3578,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1068" r:id="rId19" name="Check Box 44">
+            <control shapeId="1068" r:id="rId20" name="Check Box 44">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3559,7 +3600,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1070" r:id="rId20" name="Check Box 46">
+            <control shapeId="1070" r:id="rId21" name="Check Box 46">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3581,7 +3622,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1071" r:id="rId21" name="Check Box 47">
+            <control shapeId="1071" r:id="rId22" name="Check Box 47">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3603,7 +3644,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1072" r:id="rId22" name="Check Box 48">
+            <control shapeId="1072" r:id="rId23" name="Check Box 48">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3625,7 +3666,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1073" r:id="rId23" name="Check Box 49">
+            <control shapeId="1073" r:id="rId24" name="Check Box 49">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3647,7 +3688,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1075" r:id="rId24" name="Check Box 51">
+            <control shapeId="1075" r:id="rId25" name="Check Box 51">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3669,7 +3710,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1076" r:id="rId25" name="Check Box 52">
+            <control shapeId="1076" r:id="rId26" name="Check Box 52">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3691,7 +3732,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1077" r:id="rId26" name="Check Box 53">
+            <control shapeId="1077" r:id="rId27" name="Check Box 53">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3713,7 +3754,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1078" r:id="rId27" name="Check Box 54">
+            <control shapeId="1078" r:id="rId28" name="Check Box 54">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3735,7 +3776,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1079" r:id="rId28" name="Check Box 55">
+            <control shapeId="1079" r:id="rId29" name="Check Box 55">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>

<commit_message>
W11 moving walls+speedpowerup script start
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Status</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>script done. Needs checking later</t>
+  </si>
+  <si>
+    <t>script done.</t>
+  </si>
+  <si>
+    <t>higher wall, older looking, just make walls without diagonals, if there is time make props (eg. Painting, tables and such)</t>
+  </si>
+  <si>
+    <t>script done upto step 14</t>
   </si>
 </sst>
 </file>
@@ -319,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -413,6 +422,10 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -492,7 +505,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -981,8 +994,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1045,7 +1058,7 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2453,8 +2466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2530,7 +2543,7 @@
       </c>
       <c r="D8" s="9">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2539,7 +2552,7 @@
       </c>
       <c r="D9" s="24">
         <f>K39</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2729,7 +2742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B20" s="7">
         <v>7</v>
       </c>
@@ -2744,8 +2757,8 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G20" s="19">
-        <v>0</v>
+      <c r="G20" s="34" t="s">
+        <v>44</v>
       </c>
       <c r="J20" s="5" t="b">
         <v>0</v>
@@ -2770,7 +2783,7 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="34">
         <v>0</v>
       </c>
       <c r="J21" s="5" t="b">
@@ -2796,7 +2809,7 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="34">
         <v>0</v>
       </c>
       <c r="J22" s="5" t="b">
@@ -2822,7 +2835,7 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="34">
         <v>0</v>
       </c>
       <c r="J23" s="5" t="b">
@@ -2846,17 +2859,17 @@
       <c r="E24" s="8"/>
       <c r="F24" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G24" s="19">
-        <v>0</v>
+        <v>Done</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>43</v>
       </c>
       <c r="J24" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
@@ -2874,7 +2887,7 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="34">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="b">
@@ -2900,8 +2913,8 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G26" s="19">
-        <v>0</v>
+      <c r="G26" s="34" t="s">
+        <v>45</v>
       </c>
       <c r="J26" s="5" t="b">
         <v>0</v>
@@ -2926,7 +2939,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="34">
+        <v>0</v>
+      </c>
       <c r="J27" s="5" t="b">
         <v>0</v>
       </c>
@@ -2950,7 +2965,7 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="34"/>
       <c r="J28" s="5" t="b">
         <v>0</v>
       </c>
@@ -2974,7 +2989,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G29" s="19"/>
+      <c r="G29" s="34">
+        <v>0</v>
+      </c>
       <c r="J29" s="5" t="b">
         <v>0</v>
       </c>
@@ -3046,7 +3063,7 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="34">
         <v>0</v>
       </c>
       <c r="J32" s="5" t="b">
@@ -3206,7 +3223,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3395,8 +3412,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3417,7 +3434,7 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>21</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>

<commit_message>
hazard, powerups and tilt
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anguyen10\workspace\AGA206 GaDev\Roll-A-Ball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamoa\Desktop\fuufff\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06126FDB-9D30-4B30-B1EB-2F0029FE3DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="14295" yWindow="-10545" windowWidth="14610" windowHeight="9930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Status</t>
   </si>
@@ -134,12 +146,6 @@
     <t>[14 points minimum]</t>
   </si>
   <si>
-    <t>customise later</t>
-  </si>
-  <si>
-    <t>add texture</t>
-  </si>
-  <si>
     <t>^</t>
   </si>
   <si>
@@ -152,22 +158,31 @@
     <t>get the player and camera to sync</t>
   </si>
   <si>
-    <t>script done. Needs checking later</t>
-  </si>
-  <si>
-    <t>script done.</t>
-  </si>
-  <si>
-    <t>higher wall, older looking, just make walls without diagonals, if there is time make props (eg. Painting, tables and such)</t>
-  </si>
-  <si>
-    <t>script done upto step 14</t>
+    <t>all the assets complete</t>
+  </si>
+  <si>
+    <t>one tilt level</t>
+  </si>
+  <si>
+    <t>three hazards</t>
+  </si>
+  <si>
+    <t>they move</t>
+  </si>
+  <si>
+    <t>this waas annoying</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">script done. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -328,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,7 +356,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,22 +366,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -382,22 +393,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -405,6 +407,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -422,27 +428,12 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <strike/>
@@ -465,21 +456,12 @@
     </dxf>
     <dxf>
       <font>
-        <strike/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -513,11 +495,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,7 +519,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -585,11 +567,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -603,7 +585,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -611,7 +593,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -619,6 +601,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -667,7 +652,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
@@ -675,7 +660,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>6350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -683,6 +668,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1036"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -731,7 +719,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
@@ -739,7 +727,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>6350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -747,6 +735,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1037"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -795,7 +786,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
@@ -803,7 +794,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>6350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -811,6 +802,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1038"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -859,9 +853,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>165100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -875,6 +869,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1054"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -923,7 +920,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -939,6 +936,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1055"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -987,15 +987,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>200025</xdr:rowOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>34925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1003,6 +1003,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1056"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1051,15 +1054,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>34925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1067,6 +1070,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1057"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1115,15 +1121,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>127000</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1131,6 +1137,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1059"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1179,7 +1188,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1195,6 +1204,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1060"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1243,7 +1255,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1259,6 +1271,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1062"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1307,7 +1322,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1323,6 +1338,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1063"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1371,7 +1389,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1387,6 +1405,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1065"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1435,7 +1456,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>25</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1451,6 +1472,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1066"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1499,7 +1523,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1515,6 +1539,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1067"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1563,7 +1590,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1579,6 +1606,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1068"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1627,7 +1657,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1643,6 +1673,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1070"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1691,7 +1724,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1707,6 +1740,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1071"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1755,7 +1791,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1771,6 +1807,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1072"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1819,9 +1858,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>146050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -1835,6 +1874,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1073"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1883,7 +1925,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -1891,7 +1933,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>44450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1899,6 +1941,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1075"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1947,9 +1992,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>146050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -1963,6 +2008,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1076"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2011,9 +2059,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>146050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -2027,6 +2075,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1077"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2075,9 +2126,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>146050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -2091,6 +2142,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1078"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2139,9 +2193,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>146050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
@@ -2155,6 +2209,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1079"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2463,251 +2520,240 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="23" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="50.25" style="17" customWidth="1"/>
-    <col min="8" max="8" width="9.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.84375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.15234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.61328125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="7.4609375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="7.61328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.15234375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="50.23046875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.84375" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.125" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="5.15234375" style="2" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" style="2" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.15234375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C2" s="28" t="s">
+    <row r="2" spans="2:10" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="C2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="8" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
+      <c r="D4" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="8" t="s">
+    <row r="5" spans="2:10" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
+      <c r="D5" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="8" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="8" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="8" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="8">
         <f>K39</f>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="25" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="16" t="s">
         <v>3</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="7">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="19">
         <v>0</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="str">
+      <c r="E12" s="7"/>
+      <c r="F12" s="6" t="str">
         <f>IF(J12,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G12" s="19" t="s">
-        <v>36</v>
-      </c>
+      <c r="G12" s="17"/>
       <c r="J12" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="7">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="6">
         <v>2</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="19">
         <v>0</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7" t="str">
+      <c r="E13" s="7"/>
+      <c r="F13" s="6" t="str">
         <f>IF(J13,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G13" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="G13" s="17"/>
       <c r="J13" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="7">
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="19">
         <v>0</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7" t="str">
+      <c r="E14" s="7"/>
+      <c r="F14" s="6" t="str">
         <f>IF(J14,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G14" s="19" t="s">
-        <v>38</v>
+      <c r="G14" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="J14" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="7">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="6">
         <v>4</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="19">
         <v>0</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7" t="str">
+      <c r="E15" s="7"/>
+      <c r="F15" s="6" t="str">
         <f>IF(J15,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G15" s="19" t="s">
-        <v>38</v>
+      <c r="G15" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="J15" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="10"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="26"/>
-      <c r="J16" s="6"/>
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="20" t="s">
+      <c r="E17" s="11"/>
+      <c r="F17" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="7">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="6">
         <v>5</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="19">
         <v>2</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7" t="str">
+      <c r="E18" s="7"/>
+      <c r="F18" s="6" t="str">
         <f t="shared" ref="F18:F35" si="0">IF(J18,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G18" s="19" t="s">
-        <v>36</v>
-      </c>
+      <c r="G18" s="17"/>
       <c r="J18" s="5" t="b">
         <v>1</v>
       </c>
@@ -2716,23 +2762,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="7">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="6">
         <v>6</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="19">
         <v>2</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7" t="str">
+      <c r="E19" s="7"/>
+      <c r="F19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G19" s="19" t="s">
-        <v>42</v>
+      <c r="G19" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="J19" s="5" t="b">
         <v>1</v>
@@ -2742,76 +2788,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B20" s="7">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="6">
         <v>7</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="19">
         <v>2</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="7" t="str">
+      <c r="E20" s="7"/>
+      <c r="F20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="6">
+        <v>8</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="19">
+        <v>2</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="6">
+        <v>9</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="19">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G20" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="J20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="7">
-        <v>8</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="21">
-        <v>2</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G21" s="34">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="7">
-        <v>9</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="21">
-        <v>1</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G22" s="34">
-        <v>0</v>
-      </c>
+      <c r="G22" s="25"/>
       <c r="J22" s="5" t="b">
         <v>0</v>
       </c>
@@ -2820,24 +2864,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="7">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="6">
         <v>10</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="19">
         <v>1</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="7" t="str">
+      <c r="E23" s="7"/>
+      <c r="F23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G23" s="34">
-        <v>0</v>
-      </c>
+      <c r="G23" s="25"/>
       <c r="J23" s="5" t="b">
         <v>0</v>
       </c>
@@ -2846,22 +2888,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="7">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="6">
         <v>11</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="19">
         <v>1</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="7" t="str">
+      <c r="E24" s="7"/>
+      <c r="F24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G24" s="34" t="s">
+      <c r="G24" s="25" t="s">
         <v>43</v>
       </c>
       <c r="J24" s="5" t="b">
@@ -2872,24 +2914,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="7">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="6">
         <v>12</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="19">
         <v>1</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="7" t="str">
+      <c r="E25" s="7"/>
+      <c r="F25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G25" s="34">
-        <v>0</v>
-      </c>
+      <c r="G25" s="25"/>
       <c r="J25" s="5" t="b">
         <v>0</v>
       </c>
@@ -2898,74 +2938,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="7">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="6">
         <v>13</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="19">
         <v>1</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="7" t="str">
+      <c r="E26" s="7"/>
+      <c r="F26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="6">
+        <v>14</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="19">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="6">
+        <v>15</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="19">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G26" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="J26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="7">
-        <v>14</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="21">
-        <v>1</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G27" s="34">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="7">
-        <v>15</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="21">
-        <v>1</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G28" s="34"/>
+      <c r="G28" s="25"/>
       <c r="J28" s="5" t="b">
         <v>0</v>
       </c>
@@ -2974,24 +3014,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="7">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="6">
         <v>16</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="19">
         <v>1</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7" t="str">
+      <c r="E29" s="7"/>
+      <c r="F29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G29" s="34">
-        <v>0</v>
-      </c>
+      <c r="G29" s="25"/>
       <c r="J29" s="5" t="b">
         <v>0</v>
       </c>
@@ -3000,22 +3038,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="7">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="6">
         <v>17</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="21">
+      <c r="D30" s="19">
         <v>1</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="7" t="str">
+      <c r="E30" s="7"/>
+      <c r="F30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G30" s="19"/>
+      <c r="G30" s="17"/>
       <c r="J30" s="5" t="b">
         <v>0</v>
       </c>
@@ -3024,22 +3062,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="7">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="6">
         <v>18</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="19">
         <v>1</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="7" t="str">
+      <c r="E31" s="7"/>
+      <c r="F31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G31" s="19"/>
+      <c r="G31" s="17"/>
       <c r="J31" s="5" t="b">
         <v>0</v>
       </c>
@@ -3048,48 +3086,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="7">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="6">
         <v>19</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="19">
         <v>1</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="7" t="str">
+      <c r="E32" s="7"/>
+      <c r="F32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="6">
+        <v>20</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="19">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G32" s="34">
-        <v>0</v>
-      </c>
-      <c r="J32" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="7">
-        <v>20</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="21">
-        <v>1</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G33" s="19"/>
+      <c r="G33" s="17"/>
       <c r="J33" s="5" t="b">
         <v>0</v>
       </c>
@@ -3098,23 +3136,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="7">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="6">
         <v>21</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="19">
         <v>2</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="7" t="str">
+      <c r="E34" s="7"/>
+      <c r="F34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G34" s="19" t="s">
-        <v>41</v>
+      <c r="G34" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J34" s="5" t="b">
         <v>1</v>
@@ -3124,22 +3162,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="7">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="6">
         <v>22</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="19">
         <v>2</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="7" t="str">
+      <c r="E35" s="7"/>
+      <c r="F35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G35" s="19"/>
+      <c r="G35" s="17"/>
       <c r="J35" s="5" t="b">
         <v>0</v>
       </c>
@@ -3148,22 +3186,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="7">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="6">
         <v>23</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="19">
         <v>2</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7" t="str">
+      <c r="E36" s="7"/>
+      <c r="F36" s="6" t="str">
         <f t="shared" ref="F36:F38" si="2">IF(J36,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="17"/>
       <c r="J36" s="5" t="b">
         <v>0</v>
       </c>
@@ -3172,22 +3210,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="7">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="6">
         <v>24</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="19">
         <v>1</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="7" t="str">
+      <c r="E37" s="7"/>
+      <c r="F37" s="6" t="str">
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G37" s="19"/>
+      <c r="G37" s="17"/>
       <c r="J37" s="5" t="b">
         <v>0</v>
       </c>
@@ -3196,22 +3234,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="7">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="6">
         <v>25</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="19">
         <v>1</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7" t="str">
+      <c r="E38" s="7"/>
+      <c r="F38" s="6" t="str">
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G38" s="19"/>
+      <c r="G38" s="17"/>
       <c r="J38" s="5" t="b">
         <v>0</v>
       </c>
@@ -3220,10 +3258,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3231,33 +3269,23 @@
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="D4:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F22:F23 F26:F29 F12:F16 F34:F38">
-    <cfRule type="expression" dxfId="4" priority="10">
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThanOrEqual">
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F16">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>$F12="Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F21">
-    <cfRule type="expression" dxfId="3" priority="8">
+  <conditionalFormatting sqref="F18:F38">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>$F18="Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24:F25">
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>$F24="Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F33">
-    <cfRule type="expression" dxfId="1" priority="6">
-      <formula>$F30="Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
-      <formula>14</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
@@ -3273,7 +3301,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -3281,7 +3309,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>31750</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3295,7 +3323,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
@@ -3303,7 +3331,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3317,7 +3345,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
@@ -3325,7 +3353,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>14</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3339,7 +3367,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
@@ -3347,7 +3375,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3361,9 +3389,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>165100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
@@ -3383,7 +3411,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3405,15 +3433,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>19</xdr:row>
-                    <xdr:rowOff>200025</xdr:rowOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3427,15 +3455,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>31750</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3449,15 +3477,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>127000</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>31750</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3471,7 +3499,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>21</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3493,7 +3521,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3515,7 +3543,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3537,7 +3565,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>24</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3559,7 +3587,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>25</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3581,7 +3609,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3603,7 +3631,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3625,7 +3653,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3647,7 +3675,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3669,7 +3697,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3691,9 +3719,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>146050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
@@ -3713,7 +3741,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -3721,7 +3749,7 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>50800</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3735,9 +3763,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>146050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
@@ -3757,9 +3785,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>146050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
@@ -3779,9 +3807,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>146050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
@@ -3801,9 +3829,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>146050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>

</xml_diff>